<commit_message>
Revert "more other cows!"
This reverts commit 24002752216c01178c675cc43f2454a30e2374f3.
</commit_message>
<xml_diff>
--- a/more cows.xlsx
+++ b/more cows.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">brown cows </t>
   </si>
@@ -25,12 +25,6 @@
   </si>
   <si>
     <t>blue cows</t>
-  </si>
-  <si>
-    <t>other cows</t>
-  </si>
-  <si>
-    <t>&gt;9000</t>
   </si>
 </sst>
 </file>
@@ -369,15 +363,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,11 +381,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -400,9 +391,6 @@
       </c>
       <c r="C2">
         <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "more other cows!""
This reverts commit 443d45a6332db34850517ae552bce6800d70f23d.
</commit_message>
<xml_diff>
--- a/more cows.xlsx
+++ b/more cows.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">brown cows </t>
   </si>
@@ -25,6 +25,12 @@
   </si>
   <si>
     <t>blue cows</t>
+  </si>
+  <si>
+    <t>other cows</t>
+  </si>
+  <si>
+    <t>&gt;9000</t>
   </si>
 </sst>
 </file>
@@ -363,15 +369,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,8 +387,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -391,6 +400,9 @@
       </c>
       <c r="C2">
         <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Revert "more other cows!"""
This reverts commit 77e601476e1736e94df9db42584fc23dc59e8ccb.
</commit_message>
<xml_diff>
--- a/more cows.xlsx
+++ b/more cows.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">brown cows </t>
   </si>
@@ -25,12 +25,6 @@
   </si>
   <si>
     <t>blue cows</t>
-  </si>
-  <si>
-    <t>other cows</t>
-  </si>
-  <si>
-    <t>&gt;9000</t>
   </si>
 </sst>
 </file>
@@ -369,15 +363,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,11 +381,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -400,9 +391,6 @@
       </c>
       <c r="C2">
         <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>